<commit_message>
Update edited session - 2025-09-06T11:23:54.392Z - Cache Bust ID: 17571578343922veoky4vq
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Pediatrics_checklist1757157220874_b238c595b84321b35b8e57610c49523d4e3b9b5b5d090923e9e54f4b929bedba.xlsx
+++ b/log_history/Y4_B2526_Pediatrics_checklist1757157220874_b238c595b84321b35b8e57610c49523d4e3b9b5b5d090923e9e54f4b929bedba.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Checklist" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -436,7 +436,7 @@
         <v>13:20:02</v>
       </c>
       <c r="E2" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F2" t="str">
         <v>user@user.com</v>
@@ -444,7 +444,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>201177</v>
+        <v>201180</v>
       </c>
       <c r="B3" t="str">
         <v>Pediatrics</v>
@@ -453,38 +453,18 @@
         <v>06/09/2025</v>
       </c>
       <c r="D3" t="str">
-        <v>13:20:06</v>
+        <v>13:20:07</v>
       </c>
       <c r="E3" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F3" t="str">
-        <v>user@user.com</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>201180</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Pediatrics</v>
-      </c>
-      <c r="C4" t="str">
-        <v>06/09/2025</v>
-      </c>
-      <c r="D4" t="str">
-        <v>13:20:07</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Selection</v>
-      </c>
-      <c r="F4" t="str">
         <v>user@user.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>